<commit_message>
multiple run runner tested.
</commit_message>
<xml_diff>
--- a/conf/smoke3/smoke_featureInf.xlsx
+++ b/conf/smoke3/smoke_featureInf.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="49">
   <si>
     <t xml:space="preserve">#define default values</t>
   </si>
@@ -160,13 +160,10 @@
     <t xml:space="preserve">affirm,hypothetical</t>
   </si>
   <si>
-    <t xml:space="preserve">historical,patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">negated,certain,present,patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">negated,certain,recent,patient</t>
+    <t xml:space="preserve">affirm,historical,patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negated,certain,patient</t>
   </si>
   <si>
     <t xml:space="preserve">affirm,present,certain,patient</t>
@@ -281,10 +278,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2:I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -544,19 +541,34 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -564,13 +576,10 @@
         <v>23</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -578,13 +587,13 @@
         <v>23</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -592,19 +601,13 @@
         <v>23</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,38 +615,41 @@
         <v>23</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C17" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D17" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E17" s="0" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>41</v>
@@ -652,7 +658,7 @@
         <v>3</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>43</v>
@@ -660,66 +666,66 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="0" t="s">
+      <c r="B22" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="0" t="s">
+      <c r="B25" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="0" t="s">
+      <c r="E25" s="0" t="s">
         <v>43</v>
       </c>
     </row>
@@ -731,7 +737,7 @@
         <v>41</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>46</v>
@@ -740,20 +746,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" s="0" t="s">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="0" t="s">
         <v>43</v>
       </c>
     </row>
@@ -768,7 +774,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>43</v>
@@ -799,29 +805,29 @@
         <v>41</v>
       </c>
       <c r="C32" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="B33" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E32" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="E34" s="0" t="s">
+      <c r="E33" s="0" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix uima metaobject compare bug
</commit_message>
<xml_diff>
--- a/conf/smoke3/smoke_featureInf.xlsx
+++ b/conf/smoke3/smoke_featureInf.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="50">
   <si>
     <t xml:space="preserve">#define default values</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t xml:space="preserve">affirm,present,certain,patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -278,10 +281,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -831,6 +834,11 @@
         <v>43</v>
       </c>
     </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>